<commit_message>
Updated reference sequence declarations
</commit_message>
<xml_diff>
--- a/tabular/representative_sequences.xlsx
+++ b/tabular/representative_sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/arbovirus/Dengue/Dengue-GLUE/tabular/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD33337A-8FC1-5444-8354-EF597080F202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA28669B-7FCD-3943-939A-19922577AE26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1280" yWindow="1000" windowWidth="27140" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32907,8 +32907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACB1E95-1353-8E41-88EC-7CC1393A7FE8}">
   <dimension ref="A1:I1169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1151" workbookViewId="0">
-      <selection activeCell="E1170" sqref="E1170"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="E460" sqref="E460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>